<commit_message>
Se termin de trabjar con el almacenaje del parcial
</commit_message>
<xml_diff>
--- a/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
+++ b/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
@@ -34,7 +34,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -45,7 +44,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTI PAIS</t>
         </r>
@@ -60,7 +58,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -71,7 +68,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTI PAIS</t>
         </r>
@@ -86,7 +82,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -97,7 +92,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PONER UN VISUALIZADOR CON 4 REGIMENES</t>
         </r>
@@ -112,7 +106,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -123,7 +116,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PONER UN VISUALIZADOR CON 4 REGIMENES</t>
         </r>
@@ -138,7 +130,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -149,7 +140,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTICIUDAD</t>
         </r>
@@ -164,7 +154,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -175,7 +164,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTICIUDAD</t>
         </r>
@@ -190,7 +178,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -201,7 +188,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">EDITABLE PARA CAMBIO
 </t>
@@ -217,7 +203,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -228,7 +213,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">EDITABLE PARA CAMBIO
 </t>
@@ -836,8 +820,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * \-??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="\ * #,##0.00\ ;\ * \-#,##0.00\ ;\ * \-#\ ;\ @\ "/>
+    <numFmt numFmtId="166" formatCode="\ * #,##0.00\ ;\ * \(#,##0.00\);\ * \-#\ ;\ @\ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -845,7 +829,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -868,28 +851,24 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -897,28 +876,24 @@
       <color rgb="FF808080"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -926,7 +901,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -934,14 +908,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -949,7 +921,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -957,7 +928,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -965,27 +935,23 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -993,7 +959,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1001,7 +966,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1009,7 +973,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1017,7 +980,6 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1025,14 +987,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1202,16 +1162,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1444,15 +1400,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1154520</xdr:colOff>
+      <xdr:colOff>1155600</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>47520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1199880</xdr:colOff>
+      <xdr:colOff>1200240</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1461,8 +1417,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3110760" y="5476680"/>
-          <a:ext cx="45360" cy="323280"/>
+          <a:off x="3111840" y="5476680"/>
+          <a:ext cx="44640" cy="322920"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1470,20 +1426,15 @@
             <a:gd name="adj2" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1492,15 +1443,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1133640</xdr:colOff>
+      <xdr:colOff>1134720</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1179000</xdr:colOff>
+      <xdr:colOff>1179360</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1509,8 +1460,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3089880" y="6038640"/>
-          <a:ext cx="45360" cy="275760"/>
+          <a:off x="3090960" y="6039720"/>
+          <a:ext cx="44640" cy="275040"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1518,20 +1469,15 @@
             <a:gd name="adj2" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1546,9 +1492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>752040</xdr:colOff>
+      <xdr:colOff>751680</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>190080</xdr:rowOff>
+      <xdr:rowOff>190440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1558,7 +1504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6765840" y="10963080"/>
-          <a:ext cx="45360" cy="752040"/>
+          <a:ext cx="45000" cy="752400"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1566,20 +1512,15 @@
             <a:gd name="adj2" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
-        <a:ln/>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="minor"/>
       </xdr:style>
     </xdr:sp>
@@ -1595,8 +1536,8 @@
   </sheetPr>
   <dimension ref="A2:J179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C151" activeCellId="0" sqref="C151"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1605,7 +1546,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.53"/>
@@ -1616,21 +1559,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -1638,7 +1573,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -1646,7 +1581,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="0" t="s">
@@ -1654,7 +1589,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -1662,7 +1597,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -1670,7 +1605,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -1678,7 +1613,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -1686,7 +1621,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -1694,7 +1629,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -1702,28 +1637,28 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -1731,7 +1666,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -1739,7 +1674,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="0" t="s">
@@ -1747,53 +1682,48 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="J23" s="6" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="J23" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="0" t="s">
@@ -1806,7 +1736,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="0" t="s">
@@ -1814,10 +1744,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1827,17 +1757,17 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E35" s="0" t="s">
@@ -1845,7 +1775,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C36" s="0" t="s">
@@ -1853,7 +1783,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C37" s="0" t="s">
@@ -1864,26 +1794,26 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E40" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C41" s="0" t="s">
@@ -1892,12 +1822,12 @@
       <c r="D41" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="7" t="n">
+      <c r="E41" s="6" t="n">
         <v>2110</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C42" s="0" t="s">
@@ -1906,12 +1836,12 @@
       <c r="D42" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E42" s="8" t="n">
+      <c r="E42" s="7" t="n">
         <v>657.41</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C43" s="0" t="s">
@@ -1920,90 +1850,86 @@
       <c r="D43" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="10"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="11"/>
+      <c r="B46" s="9"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
     </row>
     <row r="48" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
+      <c r="A48" s="11"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
     </row>
     <row r="49" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="11"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="D50" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="6" t="s">
+      <c r="E50" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C51" s="0" t="s">
@@ -2012,12 +1938,12 @@
       <c r="D51" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="E51" s="7" t="n">
+      <c r="E51" s="6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="14" t="s">
         <v>71</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -2026,12 +1952,12 @@
       <c r="D52" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E52" s="7" t="n">
+      <c r="E52" s="6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="15" t="s">
+      <c r="B53" s="14" t="s">
         <v>73</v>
       </c>
       <c r="C53" s="0" t="s">
@@ -2040,12 +1966,12 @@
       <c r="D53" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="7" t="n">
+      <c r="E53" s="6" t="n">
         <v>1620</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="14" t="s">
         <v>56</v>
       </c>
       <c r="C54" s="0" t="s">
@@ -2054,12 +1980,12 @@
       <c r="D54" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E54" s="7" t="n">
+      <c r="E54" s="6" t="n">
         <v>1070</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="15" t="s">
+      <c r="B55" s="14" t="s">
         <v>76</v>
       </c>
       <c r="C55" s="0" t="s">
@@ -2068,12 +1994,12 @@
       <c r="D55" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="E55" s="7" t="n">
+      <c r="E55" s="6" t="n">
         <v>773.14</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="15" t="s">
+      <c r="B56" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -2082,217 +2008,217 @@
       <c r="D56" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="7" t="n">
+      <c r="E56" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="14"/>
+      <c r="B57" s="13"/>
       <c r="D57" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E57" s="7" t="n">
+      <c r="E57" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="14"/>
+      <c r="B58" s="13"/>
       <c r="D58" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="E58" s="7" t="n">
+      <c r="E58" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="14"/>
+      <c r="B59" s="13"/>
       <c r="D59" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="15" t="s">
+      <c r="B60" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="16" t="s">
+      <c r="D60" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="E60" s="17" t="s">
+      <c r="E60" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="15" t="s">
+      <c r="B61" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="17"/>
+      <c r="E61" s="16"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="15" t="s">
+      <c r="B62" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E62" s="17"/>
+      <c r="E62" s="16"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="15" t="s">
+      <c r="B63" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="17"/>
+      <c r="E63" s="16"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="6"/>
-      <c r="E64" s="7"/>
+      <c r="B64" s="5"/>
+      <c r="E64" s="6"/>
     </row>
     <row r="65" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E65" s="7"/>
+      <c r="E65" s="6"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C66" s="7" t="n">
+      <c r="C66" s="6" t="n">
         <v>27427.5</v>
       </c>
-      <c r="E66" s="7"/>
+      <c r="E66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="7" t="n">
+      <c r="C67" s="6" t="n">
         <v>200</v>
       </c>
-      <c r="E67" s="7"/>
+      <c r="E67" s="6"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C68" s="18" t="n">
+      <c r="C68" s="17" t="n">
         <f aca="false">((($C$66+$C$67)*2.2)*0.0018)</f>
         <v>109.4049</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E68" s="19"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="3"/>
-      <c r="C69" s="18" t="n">
+      <c r="B69" s="2"/>
+      <c r="C69" s="17" t="n">
         <f aca="false">((($C$66+$C$67)*2.2)*0.0018)</f>
         <v>109.4049</v>
       </c>
-      <c r="E69" s="7"/>
+      <c r="E69" s="6"/>
     </row>
     <row r="70" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E70" s="7"/>
+      <c r="E70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D71" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E71" s="7"/>
+      <c r="E71" s="6"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>92</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>165</v>
       </c>
-      <c r="E72" s="7"/>
+      <c r="E72" s="6"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="19" t="s">
         <v>93</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>155</v>
       </c>
-      <c r="E73" s="7"/>
+      <c r="E73" s="6"/>
     </row>
     <row r="74" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="3"/>
-      <c r="E74" s="7"/>
+      <c r="B74" s="2"/>
+      <c r="E74" s="6"/>
     </row>
     <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="3" t="s">
+      <c r="B75" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E75" s="7"/>
+      <c r="E75" s="6"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="E76" s="7"/>
+      <c r="E76" s="6"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E77" s="7"/>
+      <c r="E77" s="6"/>
     </row>
     <row r="78" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="7"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="6"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E79" s="7"/>
+      <c r="E79" s="6"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="19" t="s">
         <v>92</v>
       </c>
       <c r="C80" s="0" t="s">
@@ -2301,54 +2227,54 @@
       <c r="D80" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="E80" s="7"/>
+      <c r="E80" s="6"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="20"/>
+      <c r="B81" s="19"/>
       <c r="C81" s="0" t="s">
         <v>71</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>310</v>
       </c>
-      <c r="E81" s="7"/>
+      <c r="E81" s="6"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="20"/>
+      <c r="B82" s="19"/>
       <c r="C82" s="0" t="s">
         <v>56</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="E82" s="7"/>
+      <c r="E82" s="6"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="20"/>
+      <c r="B83" s="19"/>
       <c r="C83" s="0" t="s">
         <v>76</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="E83" s="7"/>
+      <c r="E83" s="6"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="20"/>
+      <c r="B84" s="19"/>
       <c r="C84" s="0" t="s">
         <v>59</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>330</v>
       </c>
-      <c r="E84" s="7"/>
+      <c r="E84" s="6"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="20"/>
-      <c r="E85" s="7"/>
+      <c r="B85" s="19"/>
+      <c r="E85" s="6"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="20" t="s">
+      <c r="B86" s="19" t="s">
         <v>93</v>
       </c>
       <c r="C86" s="0" t="s">
@@ -2357,118 +2283,118 @@
       <c r="D86" s="0" t="n">
         <v>195</v>
       </c>
-      <c r="E86" s="7"/>
+      <c r="E86" s="6"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="21"/>
-      <c r="E87" s="7"/>
+      <c r="B87" s="20"/>
+      <c r="E87" s="6"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E88" s="7"/>
+      <c r="E88" s="6"/>
     </row>
     <row r="89" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="7"/>
+      <c r="E89" s="6"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="C90" s="6" t="s">
+      <c r="C90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D90" s="6" t="s">
+      <c r="D90" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E90" s="6" t="s">
+      <c r="E90" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B91" s="15" t="s">
+      <c r="B91" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E91" s="23" t="s">
+      <c r="E91" s="22" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E92" s="23"/>
+      <c r="E92" s="22"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="15" t="s">
+      <c r="B93" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E93" s="23"/>
+      <c r="E93" s="22"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E94" s="23"/>
+      <c r="E94" s="22"/>
     </row>
     <row r="96" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="24" t="s">
+      <c r="B96" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E96" s="5"/>
-      <c r="F96" s="5"/>
-      <c r="G96" s="5"/>
-      <c r="I96" s="5" t="s">
+      <c r="E96" s="4"/>
+      <c r="F96" s="4"/>
+      <c r="G96" s="4"/>
+      <c r="I96" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J96" s="5"/>
+      <c r="J96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="24" t="s">
+      <c r="B97" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E97" s="5"/>
-      <c r="F97" s="5"/>
-      <c r="G97" s="5"/>
-      <c r="I97" s="5" t="s">
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="I97" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J97" s="5"/>
+      <c r="J97" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="3" t="s">
+      <c r="B99" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="25" t="s">
+      <c r="B100" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C100" s="26" t="s">
+      <c r="C100" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="15"/>
-      <c r="C101" s="5" t="s">
+      <c r="B101" s="14"/>
+      <c r="C101" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="5"/>
-      <c r="G101" s="5"/>
-      <c r="H101" s="5"/>
-      <c r="I101" s="5"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4"/>
+      <c r="H101" s="4"/>
+      <c r="I101" s="4"/>
     </row>
     <row r="103" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="23" t="s">
         <v>112</v>
       </c>
       <c r="C103" s="0" t="s">
@@ -2480,7 +2406,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="15"/>
+      <c r="B104" s="14"/>
       <c r="C104" s="0" t="s">
         <v>114</v>
       </c>
@@ -2489,20 +2415,20 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="25" t="s">
+      <c r="B107" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C107" s="26" t="s">
+      <c r="C107" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="15"/>
+      <c r="B108" s="14"/>
       <c r="C108" s="0" t="s">
         <v>116</v>
       </c>
@@ -2511,7 +2437,7 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="15"/>
+      <c r="B109" s="14"/>
       <c r="C109" s="0" t="s">
         <v>117</v>
       </c>
@@ -2520,155 +2446,152 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I111" s="5" t="s">
+      <c r="I111" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J111" s="5"/>
+      <c r="J111" s="4"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="26" t="s">
+      <c r="B112" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="C112" s="26" t="s">
+      <c r="C112" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="15" t="s">
+      <c r="B113" s="14" t="s">
         <v>119</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="4" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="15"/>
-      <c r="C114" s="27" t="s">
+      <c r="B114" s="14"/>
+      <c r="C114" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="28" t="s">
+      <c r="B116" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="I116" s="5" t="s">
+      <c r="I116" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J116" s="5"/>
+      <c r="J116" s="4"/>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C117" s="6" t="s">
+      <c r="C117" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6" t="s">
+      <c r="D117" s="5"/>
+      <c r="E117" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="15"/>
+      <c r="B118" s="14"/>
       <c r="E118" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="H118" s="5" t="s">
+      <c r="H118" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="I118" s="5"/>
-      <c r="J118" s="5"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="15"/>
+      <c r="B119" s="14"/>
       <c r="E119" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="5"/>
+      <c r="H119" s="4"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="4"/>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="15"/>
+      <c r="B120" s="14"/>
       <c r="E120" s="0" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="28" t="s">
+      <c r="B122" s="27" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="14" t="s">
+      <c r="B123" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C123" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D123" s="6" t="s">
+      <c r="D123" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="2"/>
     </row>
     <row r="126" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C126" s="13" t="s">
+      <c r="C126" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D126" s="13"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12"/>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12"/>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="14" t="s">
+      <c r="B128" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C128" s="29" t="s">
+      <c r="C128" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="D128" s="30"/>
-      <c r="E128" s="30"/>
-      <c r="F128" s="30"/>
-      <c r="G128" s="30"/>
-      <c r="H128" s="30"/>
+      <c r="D128" s="29"/>
+      <c r="E128" s="29"/>
+      <c r="F128" s="29"/>
+      <c r="G128" s="29"/>
+      <c r="H128" s="29"/>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="31" t="s">
+      <c r="B129" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="C129" s="30"/>
-      <c r="D129" s="30"/>
-      <c r="E129" s="30"/>
-      <c r="F129" s="30"/>
-      <c r="G129" s="30"/>
-      <c r="H129" s="30"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="29"/>
+      <c r="E129" s="29"/>
+      <c r="F129" s="29"/>
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="13" t="s">
         <v>136</v>
       </c>
       <c r="C130" s="0" t="s">
@@ -2676,7 +2599,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="13" t="s">
         <v>138</v>
       </c>
       <c r="C131" s="0" t="s">
@@ -2687,7 +2610,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="14" t="s">
+      <c r="B132" s="13" t="s">
         <v>141</v>
       </c>
       <c r="C132" s="0" t="s">
@@ -2695,7 +2618,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="14" t="s">
+      <c r="B133" s="13" t="s">
         <v>109</v>
       </c>
       <c r="C133" s="0" t="s">
@@ -2703,7 +2626,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="14" t="s">
+      <c r="B134" s="13" t="s">
         <v>118</v>
       </c>
       <c r="C134" s="0" t="s">
@@ -2711,7 +2634,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="14" t="s">
+      <c r="B135" s="13" t="s">
         <v>144</v>
       </c>
       <c r="C135" s="0" t="s">
@@ -2729,7 +2652,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="15" t="s">
+      <c r="B141" s="14" t="s">
         <v>147</v>
       </c>
       <c r="C141" s="0" t="s">
@@ -2737,7 +2660,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="15" t="s">
+      <c r="B142" s="14" t="s">
         <v>149</v>
       </c>
       <c r="C142" s="0" t="s">
@@ -2748,10 +2671,10 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="15" t="s">
+      <c r="B143" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="C143" s="32" t="s">
+      <c r="C143" s="31" t="s">
         <v>153</v>
       </c>
       <c r="E143" s="0" t="s">
@@ -2759,7 +2682,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="15" t="s">
+      <c r="B144" s="14" t="s">
         <v>154</v>
       </c>
       <c r="C144" s="0" t="s">
@@ -2767,12 +2690,12 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="33" t="s">
+      <c r="B145" s="32" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="15" t="s">
+      <c r="B146" s="14" t="s">
         <v>157</v>
       </c>
       <c r="C146" s="0" t="s">
@@ -2780,18 +2703,18 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="15" t="s">
+      <c r="B147" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C147" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J147" s="34" t="s">
+      <c r="J147" s="33" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="15" t="s">
+      <c r="B148" s="14" t="s">
         <v>162</v>
       </c>
       <c r="C148" s="0" t="n">
@@ -2802,7 +2725,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="35" t="s">
+      <c r="B149" s="34" t="s">
         <v>164</v>
       </c>
       <c r="C149" s="0" t="s">
@@ -2810,7 +2733,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="15" t="s">
+      <c r="B150" s="14" t="s">
         <v>166</v>
       </c>
       <c r="C150" s="0" t="s">
@@ -2818,7 +2741,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="15" t="s">
+      <c r="B151" s="14" t="s">
         <v>168</v>
       </c>
       <c r="C151" s="0" t="s">
@@ -2826,7 +2749,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="15" t="s">
+      <c r="B152" s="14" t="s">
         <v>170</v>
       </c>
       <c r="C152" s="0" t="s">
@@ -2834,7 +2757,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="36" t="s">
+      <c r="B154" s="35" t="s">
         <v>172</v>
       </c>
       <c r="C154" s="0" t="s">
@@ -2842,7 +2765,7 @@
       </c>
     </row>
     <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="28" t="s">
+      <c r="B157" s="27" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2975,7 +2898,7 @@
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="6" t="s">
+      <c r="B175" s="5" t="s">
         <v>191</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cambios en analisis de documentacion de liquidaciones aduana
</commit_message>
<xml_diff>
--- a/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
+++ b/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B40" authorId="0">
@@ -34,6 +34,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -44,6 +45,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTI PAIS</t>
         </r>
@@ -58,6 +60,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -68,6 +71,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTI PAIS</t>
         </r>
@@ -82,6 +86,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -92,6 +97,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PONER UN VISUALIZADOR CON 4 REGIMENES</t>
         </r>
@@ -106,6 +112,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -116,6 +123,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">PONER UN VISUALIZADOR CON 4 REGIMENES</t>
         </r>
@@ -130,6 +138,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -140,6 +149,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTICIUDAD</t>
         </r>
@@ -154,6 +164,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -164,6 +175,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">MULTICIUDAD</t>
         </r>
@@ -178,6 +190,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -188,6 +201,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">EDITABLE PARA CAMBIO
 </t>
@@ -203,6 +217,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Janneth Carrillo:
 </t>
@@ -213,6 +228,7 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">EDITABLE PARA CAMBIO
 </t>
@@ -224,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
   <si>
     <t xml:space="preserve">COSTOS INICIALES</t>
   </si>
@@ -310,9 +326,6 @@
     <t xml:space="preserve">JORGE Y MARIA ELENA DEPURAR SOLO LOS PROVEEDORES DE IMPORTACIONES Y CATEGORIZARLOS POR CONCEPTO DE PAGO</t>
   </si>
   <si>
-    <t xml:space="preserve">MANDAR UN PEDIDO COMPLETO CON TODOS LOS PARCIALES</t>
-  </si>
-  <si>
     <t xml:space="preserve">TABLA PEDIDO</t>
   </si>
   <si>
@@ -541,12 +554,12 @@
     <t xml:space="preserve">TASA ADUANERA</t>
   </si>
   <si>
+    <t xml:space="preserve">NO PARA REGIMEN 10</t>
+  </si>
+  <si>
     <t xml:space="preserve">TARIFA FIJA USD 40 Y EDITABLE PARA CAMBIOS POR ADMINISTRADOR</t>
   </si>
   <si>
-    <t xml:space="preserve">NO PARA REGIMEN 10</t>
-  </si>
-  <si>
     <t xml:space="preserve">CANDADO SATELITAL</t>
   </si>
   <si>
@@ -604,18 +617,18 @@
     <t xml:space="preserve">4X1000 DEL CIF ADUANA MINIMO 165</t>
   </si>
   <si>
+    <t xml:space="preserve">POR FORMULARIO EL 1ER MES USD 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A PARTIR DEL 2D0 MES SIN LOS USD 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEMORAJE</t>
+  </si>
+  <si>
     <t xml:space="preserve">LAS CONDICIONES DEBEN SER EDITABLES</t>
   </si>
   <si>
-    <t xml:space="preserve">POR FORMULARIO EL 1ER MES USD 8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A PARTIR DEL 2D0 MES SIN LOS USD 8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DEMORAJE</t>
-  </si>
-  <si>
     <t xml:space="preserve">FECHA Y NOMBRE AUTORIZADOR</t>
   </si>
   <si>
@@ -707,9 +720,6 @@
   </si>
   <si>
     <t xml:space="preserve">(FOB+SEGURO ADUANA+TRANSPORTE ADUANA+FODINFA+ARANCEL ADVALOREN+ARANCEL ESDPECIFICO+OTROS+ETIQUETAS FISCALES)/No. Botellas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CON TODOS LOS DECIMALES</t>
   </si>
   <si>
     <t xml:space="preserve">BASE ADVALOREN</t>
@@ -823,12 +833,13 @@
     <numFmt numFmtId="165" formatCode="\ * #,##0.00\ ;\ * \-#,##0.00\ ;\ * \-#\ ;\ @\ "/>
     <numFmt numFmtId="166" formatCode="\ * #,##0.00\ ;\ * \(#,##0.00\);\ * \-#\ ;\ @\ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -847,60 +858,55 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="18"/>
+      <b val="true"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -908,57 +914,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="20"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -966,6 +922,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -973,6 +930,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -980,6 +938,7 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -987,62 +946,22 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1063,7 +982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1071,23 +990,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1113,77 +1017,29 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1191,11 +1047,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1207,7 +1063,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1215,122 +1071,102 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="10" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1342,10 +1178,10 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFA9D18E"/>
@@ -1357,7 +1193,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1373,7 +1209,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
@@ -1400,15 +1236,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1155600</xdr:colOff>
+      <xdr:colOff>1155960</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>47520</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1200240</xdr:colOff>
+      <xdr:colOff>1199880</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>180000</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1417,8 +1253,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3111840" y="5476680"/>
-          <a:ext cx="44640" cy="322920"/>
+          <a:off x="3112200" y="5050080"/>
+          <a:ext cx="43920" cy="302400"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1443,15 +1279,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1134720</xdr:colOff>
+      <xdr:colOff>1135080</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>39240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1179360</xdr:colOff>
+      <xdr:colOff>1179000</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1460,8 +1296,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3090960" y="6039720"/>
-          <a:ext cx="44640" cy="275040"/>
+          <a:off x="3091320" y="5567400"/>
+          <a:ext cx="43920" cy="259200"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1488,13 +1324,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>706680</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>751680</xdr:colOff>
+      <xdr:colOff>750960</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1503,8 +1339,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6765840" y="10963080"/>
-          <a:ext cx="45000" cy="752400"/>
+          <a:off x="6765840" y="10135080"/>
+          <a:ext cx="44280" cy="690840"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1534,13 +1370,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:J179"/>
+  <dimension ref="A2:H179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.14"/>
@@ -1548,23 +1384,22 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="67.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1001" min="9" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1002" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1572,7 +1407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1596,7 +1431,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
@@ -1604,7 +1439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1612,7 +1447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1620,7 +1455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
         <v>14</v>
       </c>
@@ -1628,7 +1463,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1636,12 +1471,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1652,12 +1487,12 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1665,7 +1500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
@@ -1673,7 +1508,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="3" t="s">
         <v>23</v>
       </c>
@@ -1681,7 +1516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
@@ -1693,12 +1528,12 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1708,181 +1543,178 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="J23" s="5" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2" t="s">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="0" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="0" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="3" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="0" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3" t="s">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="3" t="s">
+      <c r="E35" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="0" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C36" s="0" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="D37" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="0" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="5" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="D41" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="E41" s="6" t="n">
         <v>2110</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="D42" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="E42" s="7" t="n">
         <v>657.41</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="D43" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="E43" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="8" t="s">
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="E45" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="9"/>
       <c r="E46" s="10"/>
     </row>
@@ -1891,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -1908,231 +1740,230 @@
       <c r="G48" s="12"/>
       <c r="H48" s="12"/>
     </row>
-    <row r="49" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E49" s="10"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="D50" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="E50" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="5" t="s">
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="14" t="s">
+      <c r="C51" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="E51" s="6" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="E52" s="6" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="D53" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="E53" s="6" t="n">
         <v>1620</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="D54" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="E54" s="6" t="n">
         <v>1070</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>77</v>
       </c>
       <c r="E55" s="6" t="n">
         <v>773.14</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="D56" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E56" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="13"/>
       <c r="D57" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E57" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="13"/>
       <c r="D58" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E58" s="6" t="n">
         <v>886.84</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="13"/>
       <c r="D59" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="15" t="s">
+      <c r="E60" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="E60" s="16" t="s">
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="16"/>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D61" s="4" t="s">
+      <c r="C62" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="16"/>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E61" s="16"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E62" s="16"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="14" t="s">
+      <c r="C63" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D63" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="E63" s="16"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="5"/>
       <c r="E64" s="6"/>
     </row>
-    <row r="65" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E65" s="6"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C66" s="6" t="n">
         <v>27427.5</v>
       </c>
       <c r="E66" s="6"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C67" s="6" t="n">
         <v>200</v>
       </c>
       <c r="E67" s="6"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="17" t="n">
         <f aca="false">((($C$66+$C$67)*2.2)*0.0018)</f>
         <v>109.4049</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E68" s="18"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B69" s="2"/>
@@ -2142,204 +1973,207 @@
       </c>
       <c r="E69" s="6"/>
     </row>
-    <row r="70" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B70" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E70" s="6"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D71" s="5" t="s">
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="E71" s="6"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="19" t="s">
-        <v>92</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>165</v>
       </c>
       <c r="E72" s="6"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>155</v>
       </c>
       <c r="E73" s="6"/>
     </row>
-    <row r="74" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="2"/>
       <c r="E74" s="6"/>
     </row>
-    <row r="75" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E75" s="6"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="19" t="s">
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="E76" s="6"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E77" s="6"/>
-    </row>
-    <row r="78" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="6"/>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B79" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D79" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C79" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D79" s="5" t="s">
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="19" t="s">
-        <v>92</v>
-      </c>
       <c r="C80" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D80" s="0" t="n">
         <v>310</v>
       </c>
       <c r="E80" s="6"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="19"/>
       <c r="C81" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D81" s="0" t="n">
         <v>310</v>
       </c>
       <c r="E81" s="6"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="19"/>
       <c r="C82" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D82" s="0" t="n">
         <v>330</v>
       </c>
       <c r="E82" s="6"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="19"/>
       <c r="C83" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D83" s="0" t="n">
         <v>330</v>
       </c>
       <c r="E83" s="6"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="19"/>
       <c r="C84" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D84" s="0" t="n">
         <v>330</v>
       </c>
       <c r="E84" s="6"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B85" s="19"/>
       <c r="E85" s="6"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D86" s="0" t="n">
         <v>195</v>
       </c>
       <c r="E86" s="6"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="20"/>
       <c r="E87" s="6"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E88" s="6"/>
     </row>
-    <row r="89" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B89" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E89" s="6"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C90" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E89" s="6"/>
-    </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="21" t="s">
+      <c r="D90" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="E91" s="22" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="14" t="s">
+      <c r="E92" s="22"/>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E92" s="22"/>
-    </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="14" t="s">
+      <c r="E93" s="22"/>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="E93" s="22"/>
-    </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="14" t="s">
+      <c r="E94" s="22"/>
+    </row>
+    <row r="96" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E94" s="22"/>
-    </row>
-    <row r="96" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="23" t="s">
+      <c r="C96" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D96" s="4" t="s">
@@ -2348,209 +2182,197 @@
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
-      <c r="I96" s="4" t="s">
+    </row>
+    <row r="97" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B97" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="J96" s="4"/>
-    </row>
-    <row r="97" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="23" t="s">
+      <c r="C97" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D97" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="E97" s="4"/>
       <c r="F97" s="4"/>
       <c r="G97" s="4"/>
-      <c r="I97" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J97" s="4"/>
-    </row>
-    <row r="99" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="99" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C100" s="25" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C100" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B101" s="14"/>
       <c r="C101" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
-      <c r="I101" s="4"/>
-    </row>
-    <row r="103" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="103" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B103" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="C103" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="C103" s="0" t="s">
-        <v>113</v>
       </c>
       <c r="D103" s="0" t="n">
         <f aca="false">D104-15</f>
         <v>234.6</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B104" s="14"/>
       <c r="C104" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D104" s="0" t="n">
         <v>249.6</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B106" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B107" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B108" s="14"/>
       <c r="C108" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D108" s="0" t="n">
         <v>660</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B109" s="14"/>
       <c r="C109" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D109" s="0" t="n">
         <v>750</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B111" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G111" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C112" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="I111" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J111" s="4"/>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C112" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>55</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="14"/>
       <c r="C114" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="D114" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D114" s="4" t="s">
+    </row>
+    <row r="116" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B116" s="27" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="27" t="s">
+      <c r="G116" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B117" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C117" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="I116" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J116" s="4"/>
-    </row>
-    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C117" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="D117" s="5"/>
       <c r="E117" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B118" s="14"/>
       <c r="E118" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="H118" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="I118" s="4"/>
-      <c r="J118" s="4"/>
-    </row>
-    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B119" s="14"/>
       <c r="E119" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H119" s="4"/>
-      <c r="I119" s="4"/>
-      <c r="J119" s="4"/>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="14"/>
       <c r="E120" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B122" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="E122" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="27" t="s">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B123" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C123" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C123" s="5" t="s">
+      <c r="D123" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="D123" s="5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
@@ -2558,7 +2380,7 @@
       <c r="G126" s="12"/>
       <c r="H126" s="12"/>
     </row>
-    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C127" s="12"/>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
@@ -2566,12 +2388,12 @@
       <c r="G127" s="12"/>
       <c r="H127" s="12"/>
     </row>
-    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B128" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C128" s="28" t="s">
         <v>133</v>
-      </c>
-      <c r="C128" s="28" t="s">
-        <v>134</v>
       </c>
       <c r="D128" s="29"/>
       <c r="E128" s="29"/>
@@ -2579,9 +2401,9 @@
       <c r="G128" s="29"/>
       <c r="H128" s="29"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B129" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C129" s="29"/>
       <c r="D129" s="29"/>
@@ -2590,336 +2412,333 @@
       <c r="G129" s="29"/>
       <c r="H129" s="29"/>
     </row>
-    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B130" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C130" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C130" s="0" t="s">
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="13" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="13" t="s">
+      <c r="C131" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C131" s="0" t="s">
+      <c r="D131" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="D131" s="0" t="s">
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B132" s="13" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="13" t="s">
+      <c r="C132" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C132" s="0" t="s">
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B133" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C133" s="0" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C133" s="0" t="s">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B134" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B135" s="13" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C134" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="13" t="s">
+      <c r="C135" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C135" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="26.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="1" t="s">
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C139" s="0" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="0" t="s">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="14" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="14" t="s">
+      <c r="C141" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C141" s="0" t="s">
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B142" s="14" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="14" t="s">
+      <c r="C142" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="E142" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="E142" s="0" t="s">
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="14" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="14" t="s">
+      <c r="C143" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C143" s="31" t="s">
+      <c r="E143" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="E143" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="14" t="s">
+      <c r="C144" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="C144" s="0" t="s">
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="32" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="32" t="s">
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="14" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="14" t="s">
+      <c r="C146" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C146" s="0" t="s">
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="14" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="14" t="s">
+      <c r="C147" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C147" s="0" t="s">
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B148" s="14" t="s">
         <v>160</v>
-      </c>
-      <c r="J147" s="33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="14" t="s">
-        <v>162</v>
       </c>
       <c r="C148" s="0" t="n">
         <v>4.33</v>
       </c>
       <c r="D148" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B149" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C149" s="0" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="34" t="s">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B150" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="C149" s="0" t="s">
+      <c r="C150" s="0" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="14" t="s">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B151" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="C150" s="0" t="s">
+      <c r="C151" s="0" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="14" t="s">
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B152" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="C151" s="0" t="s">
+      <c r="C152" s="0" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="14" t="s">
+    <row r="154" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B154" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C152" s="0" t="s">
+      <c r="C154" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="35" t="s">
+    <row r="157" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B157" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="C154" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="27" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>3</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>5</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
         <v>6</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
         <v>7</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
         <v>8</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
         <v>9</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>13</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>14</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
         <v>15</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
         <v>16</v>
       </c>
       <c r="B173" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B175" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B176" s="0" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="5" t="s">
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B177" s="0" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="0" t="s">
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B178" s="0" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="0" t="s">
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B179" s="0" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B179" s="0" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ingreso de la plantilla de impuestos
</commit_message>
<xml_diff>
--- a/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
+++ b/documentacion/analitica/Contabilidad/TABLAS PROGRAMA IMPORTACIONES.xlsx
@@ -1143,7 +1143,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1242,9 +1242,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1199880</xdr:colOff>
+      <xdr:colOff>1199520</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>174960</xdr:rowOff>
+      <xdr:rowOff>174600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1254,7 +1254,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3112200" y="5050080"/>
-          <a:ext cx="43920" cy="302400"/>
+          <a:ext cx="43560" cy="302040"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1285,9 +1285,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1179000</xdr:colOff>
+      <xdr:colOff>1178640</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1297,7 +1297,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3091320" y="5567400"/>
-          <a:ext cx="43920" cy="259200"/>
+          <a:ext cx="43560" cy="258840"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1328,9 +1328,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>750600</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>174600</xdr:rowOff>
+      <xdr:rowOff>174240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1340,7 +1340,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6765840" y="10135080"/>
-          <a:ext cx="44280" cy="690840"/>
+          <a:ext cx="43920" cy="690480"/>
         </a:xfrm>
         <a:prstGeom prst="upDownArrow">
           <a:avLst>
@@ -1372,8 +1372,8 @@
   </sheetPr>
   <dimension ref="A2:H179"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C142" activeCellId="0" sqref="C142"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A133" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C147" activeCellId="0" sqref="C147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2482,26 +2482,32 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="14" t="s">
+      <c r="B142" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="C142" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E142" s="0" t="s">
+      <c r="D142" s="5"/>
+      <c r="E142" s="5" t="s">
         <v>150</v>
       </c>
+      <c r="F142" s="5"/>
+      <c r="G142" s="5"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="14" t="s">
+      <c r="B143" s="13" t="s">
         <v>151</v>
       </c>
       <c r="C143" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="E143" s="0" t="s">
+      <c r="D143" s="5"/>
+      <c r="E143" s="5" t="s">
         <v>150</v>
       </c>
+      <c r="F143" s="5"/>
+      <c r="G143" s="5"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B144" s="14" t="s">

</xml_diff>